<commit_message>
Update profiles, oysters and clams datasets + website
</commit_message>
<xml_diff>
--- a/data/raw/2024-02-28_ksf-clam-growth.xlsx
+++ b/data/raw/2024-02-28_ksf-clam-growth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawaii0-my.sharepoint.com/personal/alemarie_hawaii_edu/Documents/Desktop/nomilo-fishpond-analysis/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{7682110A-4580-1446-B2A7-47567ED83850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7647644-F33A-459C-BC09-814E5A7116D3}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{7682110A-4580-1446-B2A7-47567ED83850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{952F6908-4989-48C1-952F-BA0FE3E7309E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{24C7CD82-E977-451A-A80B-23E335F8225B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{24C7CD82-E977-451A-A80B-23E335F8225B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Sort date</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>13/02/2024</t>
+  </si>
+  <si>
+    <t>Yellow2</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -479,11 +482,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,6 +691,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -953,18 +1046,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADAEE70-EFC3-43E0-8942-8B02D9BD4389}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="38" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" style="38" customWidth="1"/>
+    <col min="10" max="11" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -990,7 +1084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="45"/>
       <c r="B2" s="16" t="s">
         <v>6</v>
@@ -1022,7 +1116,7 @@
       <c r="K2" s="52"/>
       <c r="L2" s="43"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
         <v>14</v>
       </c>
@@ -1060,7 +1154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="40">
         <v>45089</v>
       </c>
@@ -1098,7 +1192,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="37" t="s">
         <v>13</v>
       </c>
@@ -1136,7 +1230,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="40">
         <v>45323</v>
       </c>
@@ -1174,7 +1268,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="40">
         <v>45566</v>
       </c>
@@ -1212,7 +1306,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="39" t="s">
         <v>15</v>
       </c>
@@ -1250,7 +1344,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="39" t="s">
         <v>16</v>
       </c>
@@ -1288,7 +1382,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="40">
         <v>45140</v>
       </c>
@@ -1326,7 +1420,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="41" t="s">
         <v>17</v>
       </c>
@@ -1362,6 +1456,120 @@
       </c>
       <c r="L11" s="4">
         <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="38">
+        <v>45365</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="54">
+        <v>5393</v>
+      </c>
+      <c r="D12" s="56">
+        <v>17</v>
+      </c>
+      <c r="E12" s="58">
+        <v>317.8</v>
+      </c>
+      <c r="F12" s="59">
+        <v>3800</v>
+      </c>
+      <c r="G12" s="56">
+        <v>81</v>
+      </c>
+      <c r="H12" s="60">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="I12" s="61">
+        <v>64</v>
+      </c>
+      <c r="J12" s="62">
+        <v>3.75</v>
+      </c>
+      <c r="K12" s="64">
+        <v>0.7</v>
+      </c>
+      <c r="L12" s="65">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="38">
+        <v>45370</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="54">
+        <v>22801</v>
+      </c>
+      <c r="D13" s="55">
+        <v>107</v>
+      </c>
+      <c r="E13" s="55">
+        <v>195.2</v>
+      </c>
+      <c r="F13" s="59">
+        <v>24797</v>
+      </c>
+      <c r="G13" s="55">
+        <v>234</v>
+      </c>
+      <c r="H13" s="60">
+        <v>108.8</v>
+      </c>
+      <c r="I13" s="57">
+        <v>128</v>
+      </c>
+      <c r="J13" s="62">
+        <v>1.2</v>
+      </c>
+      <c r="K13" s="63">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="L13" s="65">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="38">
+        <v>45378</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="54">
+        <v>35562</v>
+      </c>
+      <c r="D14" s="55">
+        <v>51</v>
+      </c>
+      <c r="E14" s="57">
+        <v>728.7</v>
+      </c>
+      <c r="F14" s="59">
+        <v>24869</v>
+      </c>
+      <c r="G14" s="55">
+        <v>94</v>
+      </c>
+      <c r="H14" s="60">
+        <v>272.39999999999998</v>
+      </c>
+      <c r="I14" s="57">
+        <v>43</v>
+      </c>
+      <c r="J14" s="62">
+        <v>0.85</v>
+      </c>
+      <c r="K14" s="63">
+        <v>0.7</v>
+      </c>
+      <c r="L14" s="65">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>